<commit_message>
Finished collecting data from TMDB API. Then cleaned dataframes with budgetary info and am ready to merge into large collection.
</commit_message>
<xml_diff>
--- a/dataFiles/Proj 1 Table Schema.xlsx
+++ b/dataFiles/Proj 1 Table Schema.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\Documents\FlatironRepos\Phase1\dsc-phase-1-project\dataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE28FA-B465-46C8-96DD-259B957845CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53E3ED0-E9C2-4357-A2D2-F2B9A2C1DBF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6150" windowWidth="16440" windowHeight="28440" xr2:uid="{61D52D4E-0F9A-4309-B9B4-BDE4E2BC0A12}"/>
+    <workbookView xWindow="28680" yWindow="-6150" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{61D52D4E-0F9A-4309-B9B4-BDE4E2BC0A12}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Originals Schema" sheetId="1" r:id="rId1"/>
+    <sheet name="Updated Schema" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="102">
   <si>
     <t>bom_movie_gross</t>
   </si>
@@ -319,6 +320,27 @@
   </si>
   <si>
     <t>abbreviated release region</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>budget_est</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>imdb_id</t>
+  </si>
+  <si>
+    <t>req_title</t>
+  </si>
+  <si>
+    <t>production_companies</t>
+  </si>
+  <si>
+    <t>tmdb_with_financials</t>
   </si>
 </sst>
 </file>
@@ -343,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +384,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -375,18 +427,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -697,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F2009-6673-4BA0-B6C6-6213A7049DB8}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +828,7 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
         <v>55</v>
@@ -795,7 +857,7 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>58</v>
@@ -824,7 +886,7 @@
         <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
         <v>62</v>
@@ -847,7 +909,7 @@
         <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
         <v>63</v>
@@ -870,7 +932,7 @@
         <v>47</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>20</v>
@@ -890,7 +952,7 @@
         <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
         <v>64</v>
@@ -901,12 +963,12 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -920,7 +982,7 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -933,9 +995,6 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1528,6 +1587,877 @@
         <v>93</v>
       </c>
       <c r="C79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC34D83-AABD-4756-A941-1F72303DD716}">
+  <dimension ref="A1:I84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>63</v>
+      </c>
+      <c r="B82" t="s">
+        <v>93</v>
+      </c>
+      <c r="C82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>64</v>
+      </c>
+      <c r="B84" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>